<commit_message>
Updated Excel with plan.
</commit_message>
<xml_diff>
--- a/Documentation/Datamatiker_Studie_Plan.xlsx
+++ b/Documentation/Datamatiker_Studie_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\ReEksamen\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08A3234-73D0-4A3C-8877-90C82DBF81DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4991663-A316-4904-8B04-84D1470B98E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -301,7 +301,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -324,8 +324,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -335,6 +342,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
     <fill>
@@ -353,20 +365,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="God" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -940,7 +956,7 @@
   <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V25" sqref="V25"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1063,14 +1079,16 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="6" t="s">
         <v>79</v>
       </c>
+      <c r="B19" s="7"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="6" t="s">
         <v>80</v>
       </c>
+      <c r="B20" s="7"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">

</xml_diff>